<commit_message>
Computer crashed and autosaves won't go away yet
</commit_message>
<xml_diff>
--- a/Lac_AllBounds_FLfixed14.xlsx
+++ b/Lac_AllBounds_FLfixed14.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69D429C-51C1-4EAE-92D4-50858DD709D2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A5B5A6-AC9E-4529-9F61-9935F1B018E9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{6BB9E993-27BE-4119-826B-9EA55B74D565}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6BB9E993-27BE-4119-826B-9EA55B74D565}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+  <si>
+    <t>HK-2</t>
+  </si>
+  <si>
+    <t>UMRC6</t>
+  </si>
+  <si>
+    <t>UOK262</t>
+  </si>
+  <si>
+    <t>UOK + DIDS</t>
+  </si>
+  <si>
+    <t>Kpl</t>
+  </si>
+  <si>
+    <t>Flow_Lac</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11CB92F-5B92-4350-A981-CBF419B9C2E0}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J16"/>
+      <selection activeCell="A17" sqref="A17:J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -897,6 +920,112 @@
         <v>0.1907249041854347</v>
       </c>
     </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <f>AVERAGE(B$1:B$3)</f>
+        <v>9.8222373676439996E-3</v>
+      </c>
+      <c r="D23">
+        <f>AVERAGE(B$4:B$6)</f>
+        <v>1.2749869232787816E-2</v>
+      </c>
+      <c r="E23">
+        <f>AVERAGE(B$9:B$11)</f>
+        <v>1.6686056562250012E-2</v>
+      </c>
+      <c r="F23">
+        <f>AVERAGE(B$13:B$16)</f>
+        <v>1.2858721113346901E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <f>STDEV(B$1:B$3)/SQRT(COUNT(B$1:B$3))</f>
+        <v>5.7099669301288172E-4</v>
+      </c>
+      <c r="D24">
+        <f>STDEV(B$4:B$6)/SQRT(COUNT(B$4:B$6))</f>
+        <v>5.2238862643600099E-4</v>
+      </c>
+      <c r="E24">
+        <f>STDEV(B$9:B$11)/SQRT(COUNT(B$9:B$11))</f>
+        <v>1.0191693081591985E-2</v>
+      </c>
+      <c r="F24">
+        <f>STDEV(B$13:B$16)/SQRT(COUNT(B$13:B$16))</f>
+        <v>3.0157379971263712E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="G38" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38" t="s">
+        <v>1</v>
+      </c>
+      <c r="I38" t="s">
+        <v>2</v>
+      </c>
+      <c r="J38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39">
+        <f>AVERAGE(F$1:F$3)</f>
+        <v>0.74905163230017902</v>
+      </c>
+      <c r="H39">
+        <f>AVERAGE(F$4:F$6)</f>
+        <v>0.19505065293959789</v>
+      </c>
+      <c r="I39">
+        <f>AVERAGE(F$9:F$11)</f>
+        <v>0.43625424318303274</v>
+      </c>
+      <c r="J39">
+        <f>AVERAGE(F$13:F$16)</f>
+        <v>0.30313964437902274</v>
+      </c>
+    </row>
+    <row r="40" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <f>STDEV(F$1:F$3)/SQRT(COUNT(F$1:F$3))</f>
+        <v>0.14444699553131693</v>
+      </c>
+      <c r="H40">
+        <f>STDEV(F$4:F$6)/SQRT(COUNT(F$4:F$6))</f>
+        <v>0.15258129540607809</v>
+      </c>
+      <c r="I40">
+        <f>STDEV(F$9:F$11)/SQRT(COUNT(F$9:F$11))</f>
+        <v>0.18516255965232251</v>
+      </c>
+      <c r="J40">
+        <f>STDEV(F$13:F$16)/SQRT(COUNT(F$13:F$16))</f>
+        <v>9.8130086206320369E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>